<commit_message>
activity points excel file updated
</commit_message>
<xml_diff>
--- a/activity_points.xlsx
+++ b/activity_points.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,173 +613,7 @@
       </c>
       <c r="N2" s="4" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="O2" s="4" t="n"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Sl.No</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Name of proffesional society</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Name of event</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>Start Date</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>End Date</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Duration (Days)</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>Name of the organizing instituition and Place</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
-        <is>
-          <t>Prize</t>
-        </is>
-      </c>
-      <c r="J1" s="3" t="inlineStr">
-        <is>
-          <t>Level</t>
-        </is>
-      </c>
-      <c r="K1" s="3" t="inlineStr">
-        <is>
-          <t>Cash prize amount (if any)</t>
-        </is>
-      </c>
-      <c r="L1" s="3" t="inlineStr">
-        <is>
-          <t>Certificate (File Size&lt;500kb)</t>
-        </is>
-      </c>
-      <c r="M1" s="3" t="inlineStr">
-        <is>
-          <t>Rating By Faculty</t>
-        </is>
-      </c>
-      <c r="N1" s="3" t="inlineStr">
-        <is>
-          <t>Point Status</t>
-        </is>
-      </c>
-      <c r="O1" s="3" t="inlineStr">
-        <is>
-          <t>Action</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Competitions conducted by Professional Societies</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>IEDC</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>HackS'US Edition III(24 hour hackathon)</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>15-Dec-2023</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>16-Feb-2024</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>Rajagiri School of Engineering and Technology, Kakkanad</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr">
-        <is>
-          <t>PARTICIPATION</t>
-        </is>
-      </c>
-      <c r="J2" s="4" t="inlineStr">
-        <is>
-          <t>National level</t>
-        </is>
-      </c>
-      <c r="K2" s="4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L2" s="5" t="inlineStr">
-        <is>
-          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF17/U2109053_1046030125.pdf</t>
-        </is>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
+          <t>Rejected</t>
         </is>
       </c>
       <c r="O2" s="4" t="n"/>
@@ -814,12 +648,12 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Name of professional society/ Association name/Name of Club etc.</t>
+          <t>Name of event</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>Name of event</t>
+          <t>Name of fest</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -839,36 +673,44 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Role</t>
+          <t>Name of the organizing instituition and Place</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>Documentary evidence (File Size&lt;500kb)</t>
+          <t>Prize</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Cash prize amount (if any)</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>Certificate (File Size&lt;500kb)</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
           <t>Rating By Faculty</t>
         </is>
       </c>
-      <c r="K4" s="3" t="inlineStr">
+      <c r="N4" s="3" t="inlineStr">
         <is>
           <t>Point Status</t>
         </is>
       </c>
-      <c r="L4" s="3" t="inlineStr">
+      <c r="O4" s="3" t="inlineStr">
         <is>
           <t>Action</t>
         </is>
       </c>
-      <c r="M4" s="3" t="inlineStr">
-        <is>
-          <t>Certificate (File Size&lt;500kb)</t>
-        </is>
-      </c>
-      <c r="N4" s="4" t="n"/>
-      <c r="O4" s="4" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
@@ -876,42 +718,498 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Special Initiatives</t>
+          <t>Performing Arts</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>RSET Library</t>
+          <t>Band of Brahmas</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>Annual Library Stock Verification</t>
+          <t>Eastern Group Songs</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>20-Apr-2023</t>
+          <t>4-Apr-2024</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>8-May-2023</t>
+          <t>6-Apr-2024</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>Rajagiri School of Engineering and Technology, Kakkand</t>
+        </is>
+      </c>
+      <c r="I5" s="4" t="inlineStr">
+        <is>
+          <t>SECOND</t>
+        </is>
+      </c>
+      <c r="J5" s="4" t="inlineStr">
+        <is>
+          <t>RSET</t>
+        </is>
+      </c>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="5" t="inlineStr">
+        <is>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF13/U2109053_1337838384.pdf</t>
+        </is>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="O5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Performing Arts</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Wind Instrument</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Bharatham 2024</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>4-Apr-2024</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>6-Apr-2024</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>Rajagiri School of Engineering and Technology, Kakkanad</t>
+        </is>
+      </c>
+      <c r="I6" s="4" t="inlineStr">
+        <is>
+          <t>FIRST</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <t>RSET</t>
+        </is>
+      </c>
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF13/U2109053_1337838298.pdf</t>
+        </is>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N6" s="4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="O6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Performing Arts</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Band of Brahmas</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Bharatham 2024</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>4-Apr-2024</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>6-Apr-2024</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>Rajagiri School of Engineering and Technology, Kakkanad</t>
+        </is>
+      </c>
+      <c r="I7" s="4" t="inlineStr">
+        <is>
+          <t>FIRST</t>
+        </is>
+      </c>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
+          <t>Intercollege</t>
+        </is>
+      </c>
+      <c r="K7" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" s="5" t="inlineStr">
+        <is>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF13/U2109053_1337838169.pdf</t>
+        </is>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" s="4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="O7" s="4" t="n"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L5" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L6" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L7" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Sl.No</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Name of proffesional society</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Name of event</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>End Date</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Duration (Days)</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Name of the organizing instituition and Place</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Prize</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>Cash prize amount (if any)</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Certificate (File Size&lt;500kb)</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Rating By Faculty</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Point Status</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Competitions conducted by Professional Societies</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>IEDC</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>HackS'US Edition III(24 hour hackathon)</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>15-Dec-2023</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>16-Feb-2024</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>Rajagiri School of Engineering and Technology, Kakkanad</t>
+        </is>
+      </c>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>PARTICIPATION</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>National level</t>
+        </is>
+      </c>
+      <c r="K2" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF17/U2109053_1046030125.pdf</t>
+        </is>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="O2" s="4" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="4" t="n"/>
+      <c r="I3" s="4" t="n"/>
+      <c r="J3" s="4" t="n"/>
+      <c r="K3" s="4" t="n"/>
+      <c r="L3" s="4" t="n"/>
+      <c r="M3" s="4" t="n"/>
+      <c r="N3" s="4" t="n"/>
+      <c r="O3" s="4" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Sl.No</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Name of professional society/ Association name/Name of Club etc.</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Name of event</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>End Date</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Duration (Days)</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>Documentary evidence (File Size&lt;500kb)</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>Rating By Faculty</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Point Status</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>Certificate (File Size&lt;500kb)</t>
+        </is>
+      </c>
+      <c r="N4" s="4" t="n"/>
+      <c r="O4" s="4" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Festival &amp;Technical Events</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Abhiyanthriki</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Mephestopheles</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>15-Dec-2023</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>16-Dec-2023</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>19 Days</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr">
         <is>
-          <t>Volunteer</t>
+          <t>Sub Coordinator</t>
         </is>
       </c>
       <c r="I5" s="4" t="n"/>
       <c r="J5" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K5" s="4" t="inlineStr">
         <is>
@@ -921,16 +1219,74 @@
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF26/U2109053_1569222767.pdf</t>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF26/U2109053_1337838026.pdf</t>
         </is>
       </c>
       <c r="N5" s="4" t="n"/>
       <c r="O5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Special Initiatives</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>RSET Library</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Annual Library Stock Verification</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>20-Apr-2023</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>8-May-2023</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>19 Days</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>Volunteer</t>
+        </is>
+      </c>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="n"/>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
+          <t>https://www.rajagiritech.ac.in/stud/ktu/Student/Certificate/DF26/U2109053_1569222767.pdf</t>
+        </is>
+      </c>
+      <c r="N6" s="4" t="n"/>
+      <c r="O6" s="4" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L2" r:id="rId1"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M5" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1319,7 +1675,7 @@
         </is>
       </c>
       <c r="M2" s="4" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="N2" s="4" t="inlineStr">
         <is>
@@ -2387,7 +2743,7 @@
         </is>
       </c>
       <c r="M2" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N2" s="4" t="inlineStr">
         <is>
@@ -3305,7 +3661,7 @@
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -3315,7 +3671,7 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -3335,7 +3691,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -3345,7 +3701,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -3367,7 +3723,7 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">115 </t>
+          <t xml:space="preserve">147 </t>
         </is>
       </c>
       <c r="B11" s="4" t="n"/>

</xml_diff>